<commit_message>
Add images for README description
</commit_message>
<xml_diff>
--- a/config/CoverLetterGenerator.xlsx
+++ b/config/CoverLetterGenerator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/518289307e96aafe/Documents/VBAScripts/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="999" documentId="8_{BE4BCB1A-8ED9-4CDD-88C2-821F4B2773F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71B6E2A8-E4CF-42C9-875F-EF607F405C3A}"/>
+  <xr:revisionPtr revIDLastSave="1000" documentId="8_{BE4BCB1A-8ED9-4CDD-88C2-821F4B2773F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{219A2F4F-F203-4C5D-9A38-CA5AD0BA7FF8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5BCA7793-0086-465F-9949-6E6A1564AF9F}"/>
   </bookViews>
@@ -206,10 +206,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Template file</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Tag</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -304,6 +300,10 @@
   </si>
   <si>
     <t>A motivating factor for me to apply for a role at &lt;CurCompName&gt; is that &lt;CBen&gt;.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Template file path</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -880,7 +880,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD30"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -907,7 +907,7 @@
     </row>
     <row r="2" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -921,12 +921,12 @@
     </row>
     <row r="4" spans="1:4" s="7" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -997,7 +997,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="14"/>
     </row>
@@ -1007,7 +1007,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="14"/>
     </row>
@@ -1017,7 +1017,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="14"/>
     </row>
@@ -1070,10 +1070,10 @@
         <v>11</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="14"/>
     </row>
@@ -1089,7 +1089,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D22" s="14"/>
     </row>
@@ -1099,7 +1099,7 @@
         <v>5</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="14"/>
     </row>
@@ -1109,17 +1109,17 @@
         <v>6</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D24" s="14"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" s="14"/>
     </row>
@@ -1132,10 +1132,10 @@
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D27" s="14"/>
     </row>
@@ -1199,63 +1199,63 @@
         <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="4">
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="4">
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="4">
         <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1266,64 +1266,64 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="4">
         <v>2</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="4">
         <v>3</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="4">
         <v>4</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" s="4">
         <v>5</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[WordTemplateGen] Add error handling for open Word app
</commit_message>
<xml_diff>
--- a/config/CoverLetterGenerator.xlsx
+++ b/config/CoverLetterGenerator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/518289307e96aafe/Documents/VBAScripts/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1000" documentId="8_{BE4BCB1A-8ED9-4CDD-88C2-821F4B2773F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{219A2F4F-F203-4C5D-9A38-CA5AD0BA7FF8}"/>
+  <xr:revisionPtr revIDLastSave="4275" documentId="8_{BE4BCB1A-8ED9-4CDD-88C2-821F4B2773F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FC0327E-1E9B-4246-9479-20F7B4949BDB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5BCA7793-0086-465F-9949-6E6A1564AF9F}"/>
   </bookViews>
@@ -16,18 +16,24 @@
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="PhraseConfig" sheetId="4" r:id="rId2"/>
     <sheet name="DateConfig" sheetId="3" r:id="rId3"/>
+    <sheet name="DropdownConfig" sheetId="5" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
+    <definedName name="BatchConfig" comment="Config needing change for each record of batch processing.">Variables!$D$8:$D$10</definedName>
     <definedName name="CompName" comment="Company name to use in file name.">Variables!$D$8</definedName>
-    <definedName name="Content" comment="All content">Variables!$D$8:$D$27</definedName>
+    <definedName name="Content" comment="All content">Variables!$D$8:$D$29</definedName>
     <definedName name="Date" comment="Date tag.">Variables!$C$6</definedName>
-    <definedName name="FileNamePrefix" comment="Prefix in file name (describe the document you are creating)">Variables!$D$4</definedName>
-    <definedName name="Phrases" comment="Stock phrases to use in letter.">PhraseConfig!$D:$D</definedName>
+    <definedName name="FeedPath" comment="Excel file path containing job listings to feed to batch process.">Variables!$D$3</definedName>
+    <definedName name="FileNamePrefix" comment="Prefix in file name (describe the document you are creating)">Variables!$D$5</definedName>
+    <definedName name="JobTitle" comment="Job title">Variables!$D$9</definedName>
+    <definedName name="ListingPath" comment="Project list Excel path">Variables!$D$4</definedName>
+    <definedName name="ListItem" comment="Matching list items to L tags.">PhraseConfig!$C:$C</definedName>
+    <definedName name="Phrases" comment="Stock phrases to use in letter.">PhraseConfig!$E:$E</definedName>
     <definedName name="PhraseTags" comment="Tags in PhraseConfig sheet">PhraseConfig!$B:$B</definedName>
-    <definedName name="Tags" comment="All tag names to search for">Variables!$C$8:$C$27</definedName>
+    <definedName name="Tags" comment="All tag names to search for">Variables!$C$7:$C$29</definedName>
     <definedName name="Template" comment="File path of template.">Variables!$D$2</definedName>
     <definedName name="UsedDateConfig" comment="Date config table for lookup.">DateConfig!$A$1:$B$10</definedName>
   </definedNames>
@@ -79,12 +85,372 @@
         </r>
       </text>
     </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{1EA9E1CC-2DE3-4A0C-B5E6-6A38340BC1E1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kei Tsun Adriel Yeung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Word template for filling in.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{DD3D2E49-BBEC-4672-8166-44AA81168768}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kei Tsun Adriel Yeung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Excel file path containing all jobs to be generated (with status = "Prepare")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{AAE7EDFA-BEE3-433D-B7F7-A6F22EFDA846}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kei Tsun Adriel Yeung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Excel file path containing all project experience</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{5BE77B5F-5813-4C4F-95FE-4DA8A78C096C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kei Tsun Adriel Yeung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This will be added at the start of the file name.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{EA2E3FD3-F7DC-4031-8DDC-EE9DE911D1AE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kei Tsun Adriel Yeung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+System will apply date of today.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{87EF08E7-E62F-427E-91AF-D1DAE8117FA5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kei Tsun Adriel Yeung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Current company name applying for.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{D00B459A-239E-4620-9649-04777CD388F4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kei Tsun Adriel Yeung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Current job title applying for.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{0882A2B4-FD06-4215-A1C2-1A6DB1BE19EB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kei Tsun Adriel Yeung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Do not fill in. For program use only. Fill in skills in L&lt;Skills&gt; field instead.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{A6627627-F6CE-4788-B181-C102B9378E07}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kei Tsun Adriel Yeung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Knowledge of job opening</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{E5B9952F-9E12-4DBB-9628-CC6EE8D0305B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kei Tsun Adriel Yeung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Company benefit</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="0" shapeId="0" xr:uid="{5E9BD7C3-5CAB-493A-87F6-42A96382E888}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kei Tsun Adriel Yeung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Company working in now.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{CD4D72FC-3250-474D-B2A5-386C8EDADD7C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kei Tsun Adriel Yeung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Job title working in now.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{3D367518-1621-49C5-94B5-F9564E2A5C3D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kei Tsun Adriel Yeung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Work experience in years.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{71222AEC-5967-42C6-8882-C60D470E55B3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kei Tsun Adriel Yeung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skills.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{901E535C-DF4C-4AEC-8624-07B033572EB0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kei Tsun Adriel Yeung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Matching experience. If prefer to draw matching experience from Excel config, leave blank.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="80">
   <si>
     <t>Company name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -112,6 +478,16 @@
     <t>Matching experience 3</t>
   </si>
   <si>
+    <t>Matching certification 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Matching certification 2</t>
+  </si>
+  <si>
+    <t>Matching certification 3</t>
+  </si>
+  <si>
     <t>Previous job info</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -245,19 +621,94 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>P&lt;Cert&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Matching Experience</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;Exp&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Matching Certification</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;Cert&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;Lang&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Languages (level)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I had previous experience in &lt;Exp&gt;.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>My work as &lt;PrevJobTitle&gt; in &lt;PrevCompName&gt; has involved work in &lt;Exp&gt;.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I have been tasked with working in &lt;Exp&gt;.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For my last experience, I have worked in &lt;Exp&gt;.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Matching experience 4</t>
+  </si>
+  <si>
+    <t>Working in &lt;Exp&gt; can demonstrate the above skills.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A motivating factor for me to apply for a role at &lt;CurCompName&gt; is that &lt;CBen&gt;.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Template file path</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Job name log</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Project list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Document type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Matching skills 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Matching skills 2</t>
+  </si>
+  <si>
+    <t>Matching skills 3</t>
+  </si>
+  <si>
+    <t>Matching skills 4</t>
+  </si>
+  <si>
     <t>&lt;Skill&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Matching Experience</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;Exp&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;Lang&gt;</t>
+  </si>
+  <si>
+    <t>L&lt;Skill&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -265,45 +716,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Languages (level)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CoverLetter_</t>
-  </si>
-  <si>
-    <t>Output file name prefix</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>I had previous experience in &lt;Exp&gt;.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>My work as &lt;PrevJobTitle&gt; in &lt;PrevCompName&gt; has involved work in &lt;Exp&gt;.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>I have been tasked with working in &lt;Exp&gt;.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>For my last experience, I have worked in &lt;Exp&gt;.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Matching experience 4</t>
-  </si>
-  <si>
-    <t>Working in &lt;Exp&gt; can demonstrate the above skills.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A motivating factor for me to apply for a role at &lt;CurCompName&gt; is that &lt;CBen&gt;.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Template file path</t>
+    <t>My work using &lt;Skill&gt; involved &lt;ListItem&gt;.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ListItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Required skills</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B&lt;Skill&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the Internet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a Career Fair</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>my friend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>my family</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;Name&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Signature Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -450,13 +899,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -467,6 +910,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,6 +938,10 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -504,7 +957,7 @@
           <xdr:col>6</xdr:col>
           <xdr:colOff>495300</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>144780</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -550,7 +1003,76 @@
                   <a:latin typeface="Arial"/>
                   <a:cs typeface="Arial"/>
                 </a:rPr>
-                <a:t>Generate</a:t>
+                <a:t>Generate single</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>487680</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>304800</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>480060</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>144780</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1027" name="Button 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1027"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="zh-TW" altLang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial"/>
+                  <a:cs typeface="Arial"/>
+                </a:rPr>
+                <a:t>Generate batch</a:t>
               </a:r>
             </a:p>
           </xdr:txBody>
@@ -570,7 +1092,8 @@
       <sheetName val="Sheet1"/>
     </sheetNames>
     <definedNames>
-      <definedName name="ReplaceTagsWithContent"/>
+      <definedName name="Batch_ReplaceTagsWithContent"/>
+      <definedName name="Single_ReplaceTagsWithContent"/>
     </definedNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -877,81 +1400,86 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D38B58-4AC7-4C0E-A15B-CEB815765993}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D7" activeCellId="1" sqref="D2:D5 D7:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.25" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27.75" style="1" customWidth="1"/>
-    <col min="4" max="4" width="46.625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="46.625" style="13" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
+      <c r="A3" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="1:4" s="7" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
-        <v>49</v>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="D4" s="15"/>
     </row>
     <row r="5" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
+      <c r="A5" s="14" t="s">
+        <v>62</v>
+      </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="11"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>25</v>
+        <v>17</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="13"/>
+      <c r="C7" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -961,9 +1489,9 @@
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="14"/>
+        <v>26</v>
+      </c>
+      <c r="D8" s="12"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
@@ -971,117 +1499,133 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="D9" s="12"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="14"/>
+        <v>73</v>
+      </c>
+      <c r="D10" s="12"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="13"/>
+      <c r="B11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="12"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="14"/>
+        <v>39</v>
+      </c>
+      <c r="D12" s="12"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="14"/>
+        <v>39</v>
+      </c>
+      <c r="D13" s="12"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="14"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="13"/>
+      <c r="B15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="12"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="14"/>
+        <v>19</v>
+      </c>
+      <c r="D16" s="12"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="14"/>
+        <v>18</v>
+      </c>
+      <c r="D17" s="12"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
+      <c r="A18" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="B18" s="4" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="14"/>
+        <v>68</v>
+      </c>
+      <c r="D18" s="12"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="13"/>
+      <c r="B19" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="12"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="14"/>
+        <v>68</v>
+      </c>
+      <c r="D20" s="12"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="13"/>
+      <c r="B21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="12"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
@@ -1089,9 +1633,9 @@
         <v>4</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="14"/>
+        <v>44</v>
+      </c>
+      <c r="D22" s="12"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
@@ -1099,9 +1643,9 @@
         <v>5</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="14"/>
+        <v>44</v>
+      </c>
+      <c r="D23" s="12"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
@@ -1109,35 +1653,59 @@
         <v>6</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="14"/>
+        <v>44</v>
+      </c>
+      <c r="D24" s="12"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="14"/>
+        <v>44</v>
+      </c>
+      <c r="D25" s="12"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="13"/>
+      <c r="B26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="12"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="14"/>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
+      <c r="B28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="12"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
+      <c r="B29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1151,7 +1719,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="1025" r:id="rId4" name="Button 1">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!ReplaceTagsWithContent">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!Single_ReplaceTagsWithContent">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
@@ -1163,6 +1731,28 @@
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>495300</xdr:colOff>
                     <xdr:row>2</xdr:row>
+                    <xdr:rowOff>160020</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1027" r:id="rId5" name="Button 3">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!Batch_ReplaceTagsWithContent">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>487680</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>304800</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>6</xdr:col>
+                    <xdr:colOff>480060</xdr:colOff>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>144780</xdr:rowOff>
                   </to>
                 </anchor>
@@ -1173,164 +1763,295 @@
       </controls>
     </mc:Choice>
   </mc:AlternateContent>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value not allowed" error="Please select from dropdown" promptTitle="Select from dropdown" prompt="Please select from dropdown." xr:uid="{FA91737E-27B5-4364-835B-1BD66E8475BD}">
+          <x14:formula1>
+            <xm:f>DropdownConfig!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>D11</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963A5ED5-A5D3-4C61-B0D6-EFA36C042815}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="90.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="1"/>
+    <col min="3" max="3" width="10.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="90.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="4">
+        <v>69</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="16">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="16">
+        <v>2</v>
+      </c>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="16">
+        <v>3</v>
+      </c>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="16">
+        <v>4</v>
+      </c>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="4">
-        <v>3</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="4">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4">
         <v>1</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="4">
+        <v>40</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4">
         <v>2</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="4">
+        <v>40</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4">
         <v>3</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="4">
+        <v>40</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4">
         <v>4</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4">
+        <v>2</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4">
+        <v>3</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4">
+        <v>4</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4">
         <v>5</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4">
+        <v>2</v>
+      </c>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4">
+        <v>3</v>
+      </c>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4">
+        <v>4</v>
+      </c>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1357,10 +2078,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1368,7 +2089,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1376,7 +2097,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1384,7 +2105,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1392,7 +2113,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1400,7 +2121,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1408,7 +2129,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1416,7 +2137,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1424,7 +2145,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1432,7 +2153,48 @@
         <v>31</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E145B83-064D-405F-A499-09E290105D1E}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[WordTemplateGen] Add image files and update config files
</commit_message>
<xml_diff>
--- a/config/CoverLetterGenerator.xlsx
+++ b/config/CoverLetterGenerator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/518289307e96aafe/Documents/VBAScripts/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4275" documentId="8_{BE4BCB1A-8ED9-4CDD-88C2-821F4B2773F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FC0327E-1E9B-4246-9479-20F7B4949BDB}"/>
+  <xr:revisionPtr revIDLastSave="4293" documentId="8_{BE4BCB1A-8ED9-4CDD-88C2-821F4B2773F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7E4D431-E6B3-4B69-B51A-44BD18337A3F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5BCA7793-0086-465F-9949-6E6A1564AF9F}"/>
+    <workbookView xWindow="336" yWindow="0" windowWidth="12072" windowHeight="11712" xr2:uid="{5BCA7793-0086-465F-9949-6E6A1564AF9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -301,7 +301,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{E5B9952F-9E12-4DBB-9628-CC6EE8D0305B}">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{F1EDBCA5-5777-4125-A1B5-2B8CB7911847}">
       <text>
         <r>
           <rPr>
@@ -349,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{CD4D72FC-3250-474D-B2A5-386C8EDADD7C}">
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{93712934-C1BE-4CCD-8803-729AB98F5124}">
       <text>
         <r>
           <rPr>
@@ -369,7 +369,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Job title working in now.</t>
+Current job title applying for.</t>
         </r>
       </text>
     </comment>
@@ -421,7 +421,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{901E535C-DF4C-4AEC-8624-07B033572EB0}">
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{9F0AC999-FF5C-4725-AB27-4D31764B7758}">
       <text>
         <r>
           <rPr>
@@ -450,7 +450,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
   <si>
     <t>Company name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -753,6 +753,61 @@
   </si>
   <si>
     <t>Signature Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>config/ProjectList.xlsx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>config/JobApplication.xlsx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>config/CoverLetterTemplate.docx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adrielyeung</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GitHub</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>the Internet</t>
+  </si>
+  <si>
+    <t>Prev Company</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;CurCompName&gt; has a lot of large-scale applications</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>there are a lot of development opportunities</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>an agile squad to deliver Java RESTful APIs and microservices, for a client's cloud migration project to Microsoft Azure database</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>using automation deployment tool Jenkins to deploy the microservices</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>collaborating with business analysts, software testers and users to ensure delivery of the software in tough deadlines, through participation in regular standup meetings and sprint reviews</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>English, Chinese</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1402,8 +1457,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" activeCellId="1" sqref="D2:D5 D7:D29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1434,14 +1489,18 @@
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="8"/>
+      <c r="D2" s="8" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="3" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>60</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="D3" s="15"/>
+      <c r="D3" s="15" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="4" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
@@ -1449,7 +1508,9 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="15"/>
+      <c r="D4" s="15" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="5" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
@@ -1479,7 +1540,9 @@
       <c r="C7" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="12"/>
+      <c r="D7" s="12" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -1491,7 +1554,9 @@
       <c r="C8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="12"/>
+      <c r="D8" s="12" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
@@ -1501,7 +1566,9 @@
       <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="12"/>
+      <c r="D9" s="12" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
@@ -1521,9 +1588,11 @@
       <c r="C11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="12"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
         <v>11</v>
@@ -1531,7 +1600,9 @@
       <c r="C12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="12"/>
+      <c r="D12" s="12" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
@@ -1541,7 +1612,9 @@
       <c r="C13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="12"/>
+      <c r="D13" s="12" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
@@ -1563,7 +1636,9 @@
       <c r="C15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
@@ -1573,7 +1648,9 @@
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="12"/>
+      <c r="D16" s="12" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
@@ -1583,7 +1660,9 @@
       <c r="C17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="12"/>
+      <c r="D17" s="12">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -1627,7 +1706,7 @@
       </c>
       <c r="D21" s="12"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="4" t="s">
         <v>4</v>
@@ -1635,9 +1714,11 @@
       <c r="C22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="12"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D22" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
         <v>5</v>
@@ -1645,9 +1726,11 @@
       <c r="C23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D23" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="69" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
         <v>6</v>
@@ -1655,7 +1738,9 @@
       <c r="C24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="12"/>
+      <c r="D24" s="12" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
@@ -1705,7 +1790,9 @@
       <c r="C29" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="12"/>
+      <c r="D29" s="12" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
[WordTemplateGen] Update config files
</commit_message>
<xml_diff>
--- a/config/CoverLetterGenerator.xlsx
+++ b/config/CoverLetterGenerator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/518289307e96aafe/Documents/VBAScripts/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4293" documentId="8_{BE4BCB1A-8ED9-4CDD-88C2-821F4B2773F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7E4D431-E6B3-4B69-B51A-44BD18337A3F}"/>
+  <xr:revisionPtr revIDLastSave="6464" documentId="8_{BE4BCB1A-8ED9-4CDD-88C2-821F4B2773F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7B5828B-44BA-45E3-96DA-91BDF48309CA}"/>
   <bookViews>
-    <workbookView xWindow="336" yWindow="0" windowWidth="12072" windowHeight="11712" xr2:uid="{5BCA7793-0086-465F-9949-6E6A1564AF9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5BCA7793-0086-465F-9949-6E6A1564AF9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,6 @@
   <definedNames>
     <definedName name="BatchConfig" comment="Config needing change for each record of batch processing.">Variables!$D$8:$D$10</definedName>
     <definedName name="CompName" comment="Company name to use in file name.">Variables!$D$8</definedName>
-    <definedName name="Content" comment="All content">Variables!$D$8:$D$29</definedName>
     <definedName name="Date" comment="Date tag.">Variables!$C$6</definedName>
     <definedName name="FeedPath" comment="Excel file path containing job listings to feed to batch process.">Variables!$D$3</definedName>
     <definedName name="FileNamePrefix" comment="Prefix in file name (describe the document you are creating)">Variables!$D$5</definedName>
@@ -301,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{F1EDBCA5-5777-4125-A1B5-2B8CB7911847}">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{E5B9952F-9E12-4DBB-9628-CC6EE8D0305B}">
       <text>
         <r>
           <rPr>
@@ -349,7 +348,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{93712934-C1BE-4CCD-8803-729AB98F5124}">
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{CD4D72FC-3250-474D-B2A5-386C8EDADD7C}">
       <text>
         <r>
           <rPr>
@@ -369,7 +368,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Current job title applying for.</t>
+Job title working in now.</t>
         </r>
       </text>
     </comment>
@@ -421,7 +420,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{9F0AC999-FF5C-4725-AB27-4D31764B7758}">
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{1C13996B-B955-4A68-9678-42B07E1099F8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Kei Tsun Adriel Yeung:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If Project list is defined, fill in number of relevant items to include for this skill. (if found)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{901E535C-DF4C-4AEC-8624-07B033572EB0}">
       <text>
         <r>
           <rPr>
@@ -450,7 +473,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="103">
   <si>
     <t>Company name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -528,9 +551,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;PrevCompName&gt;</t>
-  </si>
-  <si>
     <t>Category</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -547,13 +567,13 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;CurCompName&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;JobKnowledge&gt;</t>
   </si>
   <si>
+    <t>IT Consultant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Auto-generated</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -590,6 +610,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>there are a lot of development opportunities</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>#</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -606,17 +630,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>One of the reasons for attracting me to &lt;CurCompName&gt; is that &lt;CBen&gt;.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>From my study of &lt;CurCompName&gt;, I have found out that &lt;CBen&gt;.</t>
-  </si>
-  <si>
-    <t>One of the benefits for working at &lt;CurCompName&gt; is that &lt;CBen&gt;.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>P&lt;Exp&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -653,7 +666,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>My work as &lt;PrevJobTitle&gt; in &lt;PrevCompName&gt; has involved work in &lt;Exp&gt;.</t>
+    <t>using automation deployment tool Jenkins to deploy the microservices</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -665,14 +678,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>collaborating with business analysts, software testers and users to ensure delivery of the software in tough deadlines, through participation in regular standup meetings and sprint reviews</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Matching experience 4</t>
   </si>
   <si>
+    <t>leading discussions with the developer teams and translated their ideas for business users</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Working in &lt;Exp&gt; can demonstrate the above skills.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>A motivating factor for me to apply for a role at &lt;CurCompName&gt; is that &lt;CBen&gt;.</t>
+    <t>an agile squad to deliver Java RESTful APIs and microservices, for a client's cloud migration project to Microsoft Azure database</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -688,6 +709,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>CoverLetter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Document type</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -716,14 +741,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>My work using &lt;Skill&gt; involved &lt;ListItem&gt;.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ListItem</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>English (IELTS overall grade 8.0), Mandarin (PSC 二級甲等), Cantonese (native)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Required skills</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -732,6 +757,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>VBA Developer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Batch, VBA, Excel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Batch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VBA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Excel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>the Internet</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -756,58 +801,70 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>I have equipped skills in &lt;Skill&gt; through &lt;ListDesc&gt; during my role as &lt;ListJobTitle&gt; at &lt;ListComp&gt;.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For &lt;Skill&gt;, my work as &lt;ListJobTitle&gt; at &lt;ListComp&gt; involving &lt;ListDesc&gt;.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I have used &lt;Skill&gt; as &lt;ListJobTitle&gt; at &lt;ListComp&gt;, my work during which involving &lt;ListDesc&gt;.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I have previous experience in &lt;Skill&gt; as &lt;ListJobTitle&gt; at &lt;ListComp&gt; in &lt;ListDesc&gt;.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;PrevComp&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;CurComp&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;CurComp&gt; has a lot of large-scale projects</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>One of the reasons for attracting me to &lt;CurComp&gt; is that &lt;CBen&gt;.</t>
+  </si>
+  <si>
+    <t>From my study of &lt;CurComp&gt;, I have found out that &lt;CBen&gt;.</t>
+  </si>
+  <si>
+    <t>One of the benefits for working at &lt;CurComp&gt; is that &lt;CBen&gt;.</t>
+  </si>
+  <si>
+    <t>A motivating factor for me to apply for a role at &lt;CurComp&gt; is that &lt;CBen&gt;.</t>
+  </si>
+  <si>
+    <t>My work as &lt;PrevJobTitle&gt; in &lt;PrevComp&gt; has involved work in &lt;Exp&gt;.</t>
+  </si>
+  <si>
+    <t># of List Items</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>config/CoverLetterTemplate.docx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>config/CoverLetterGenerator.xlsx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>config/ProjectList.xlsx</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>config/JobApplication.xlsx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>config/CoverLetterTemplate.docx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>adrielyeung</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Software Engineer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GitHub</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>the Internet</t>
-  </si>
-  <si>
-    <t>Prev Company</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;CurCompName&gt; has a lot of large-scale applications</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>there are a lot of development opportunities</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>an agile squad to deliver Java RESTful APIs and microservices, for a client's cloud migration project to Microsoft Azure database</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>using automation deployment tool Jenkins to deploy the microservices</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>collaborating with business analysts, software testers and users to ensure delivery of the software in tough deadlines, through participation in regular standup meetings and sprint reviews</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>English, Chinese</t>
+    <t>Current Company</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Previous Company</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -920,7 +977,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -969,9 +1026,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1003,13 +1057,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>4</xdr:col>
+          <xdr:col>5</xdr:col>
           <xdr:colOff>502920</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>15240</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>495300</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>160020</xdr:rowOff>
@@ -1072,13 +1126,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor>
         <xdr:from>
-          <xdr:col>4</xdr:col>
+          <xdr:col>5</xdr:col>
           <xdr:colOff>487680</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>304800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
+          <xdr:col>7</xdr:col>
           <xdr:colOff>480060</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>144780</xdr:rowOff>
@@ -1147,7 +1201,7 @@
       <sheetName val="Sheet1"/>
     </sheetNames>
     <definedNames>
-      <definedName name="Batch_ReplaceTagsWithContent"/>
+      <definedName name="Batch_ReplaceTagsWithContent_Generator"/>
       <definedName name="Single_ReplaceTagsWithContent"/>
     </definedNames>
     <sheetDataSet>
@@ -1455,10 +1509,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D38B58-4AC7-4C0E-A15B-CEB815765993}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1466,61 +1520,71 @@
     <col min="1" max="1" width="24.25" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="27.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="46.625" style="13" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="1"/>
+    <col min="5" max="5" width="17.875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="7" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:5" s="7" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="6"/>
       <c r="D3" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5" s="7" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" s="7" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>62</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="D5" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -1529,22 +1593,22 @@
         <v>17</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7" s="12"/>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>3</v>
       </c>
@@ -1552,13 +1616,14 @@
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>1</v>
@@ -1567,10 +1632,11 @@
         <v>20</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="E9" s="11"/>
+    </row>
+    <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="4" t="s">
         <v>72</v>
@@ -1578,21 +1644,25 @@
       <c r="C10" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="11"/>
+    </row>
+    <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
         <v>11</v>
@@ -1601,10 +1671,11 @@
         <v>39</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="4" t="s">
         <v>12</v>
@@ -1613,10 +1684,11 @@
         <v>39</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="4" t="s">
         <v>13</v>
@@ -1625,8 +1697,9 @@
         <v>39</v>
       </c>
       <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E14" s="11"/>
+    </row>
+    <row r="15" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
@@ -1634,13 +1707,14 @@
         <v>0</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>21</v>
+        <v>89</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
         <v>1</v>
@@ -1649,10 +1723,11 @@
         <v>19</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="E16" s="11"/>
+    </row>
+    <row r="17" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="4" t="s">
         <v>15</v>
@@ -1663,8 +1738,9 @@
       <c r="D17" s="12">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="11"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
@@ -1674,9 +1750,14 @@
       <c r="C18" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="12"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="4" t="s">
         <v>64</v>
@@ -1684,9 +1765,14 @@
       <c r="C19" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="12"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D19" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="4" t="s">
         <v>65</v>
@@ -1694,9 +1780,14 @@
       <c r="C20" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="12"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D20" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
         <v>66</v>
@@ -1705,94 +1796,107 @@
         <v>68</v>
       </c>
       <c r="D21" s="12"/>
-    </row>
-    <row r="22" spans="1:4" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="E21" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="E22" s="11"/>
+    </row>
+    <row r="23" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="69" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="E23" s="11"/>
+    </row>
+    <row r="24" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="E24" s="11"/>
+    </row>
+    <row r="25" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="12"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="11"/>
+    </row>
+    <row r="26" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D26" s="12"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="11"/>
+    </row>
+    <row r="27" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D27" s="12"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27" s="11"/>
+    </row>
+    <row r="28" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D28" s="12"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28" s="11"/>
+    </row>
+    <row r="29" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>93</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="E29" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1809,13 +1913,13 @@
               <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!Single_ReplaceTagsWithContent">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>4</xdr:col>
+                    <xdr:col>5</xdr:col>
                     <xdr:colOff>502920</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>15240</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>495300</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>160020</xdr:rowOff>
@@ -1828,16 +1932,16 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="1027" r:id="rId5" name="Button 3">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!Batch_ReplaceTagsWithContent">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[1]!Batch_ReplaceTagsWithContent_Generator">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
-                    <xdr:col>4</xdr:col>
+                    <xdr:col>5</xdr:col>
                     <xdr:colOff>487680</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>304800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>7</xdr:col>
                     <xdr:colOff>480060</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>144780</xdr:rowOff>
@@ -1868,277 +1972,267 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963A5ED5-A5D3-4C61-B0D6-EFA36C042815}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="90.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="24" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="3" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="90.375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="16">
+      <c r="C2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="8">
         <v>1</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="16">
+      <c r="E2" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="10"/>
+      <c r="B3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="8">
         <v>2</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="8" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="16">
+      <c r="A4" s="10"/>
+      <c r="B4" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="8">
         <v>3</v>
       </c>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="16">
+      <c r="E4" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="8">
         <v>4</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="A6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8">
+        <v>3</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8">
+        <v>4</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8">
         <v>1</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4">
+      <c r="E10" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8">
         <v>2</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4">
+      <c r="E11" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8">
         <v>3</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4">
+      <c r="E12" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8">
         <v>4</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="E13" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8">
+        <v>5</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4">
+      <c r="C15" s="8"/>
+      <c r="D15" s="8">
         <v>1</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4">
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8">
         <v>2</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4">
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8">
         <v>3</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4">
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8">
         <v>4</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4">
-        <v>5</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4">
-        <v>2</v>
-      </c>
-      <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4">
-        <v>3</v>
-      </c>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4">
-        <v>4</v>
-      </c>
-      <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="E18" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2165,10 +2259,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2176,7 +2270,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2184,7 +2278,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2192,7 +2286,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2200,7 +2294,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2208,7 +2302,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2216,7 +2310,7 @@
         <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2224,7 +2318,7 @@
         <v>23</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2232,7 +2326,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2240,7 +2334,7 @@
         <v>31</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2266,22 +2360,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>